<commit_message>
Penambahan File Presentasi dan Perbaikan BurnDownChart
</commit_message>
<xml_diff>
--- a/technoterburndownchart.xlsx
+++ b/technoterburndownchart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\[CAMPUS]\[BAHANKULIAH]\[IV]\[TKPPL][AXA]\[TUGASBESAR]\technoter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\[CAMPUS]\[BAHANKULIAH]\[IV]\[TKPPL][AXA]\technoter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -109,9 +109,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +132,22 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,20 +223,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -234,16 +242,23 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,11 +632,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="290113560"/>
-        <c:axId val="290114736"/>
+        <c:axId val="287722808"/>
+        <c:axId val="287723984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="290113560"/>
+        <c:axId val="287722808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +678,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290114736"/>
+        <c:crossAx val="287723984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -671,7 +686,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290114736"/>
+        <c:axId val="287723984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -721,7 +736,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="290113560"/>
+        <c:crossAx val="287722808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1652,561 +1667,561 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41" style="4" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
     <col min="5" max="14" width="13.5703125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="13.5703125" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="4"/>
+    <col min="15" max="16" width="13.5703125" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:16" s="9" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="8">
         <v>41804</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <v>41803</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="8">
         <v>41802</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="8">
         <v>41801</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="8">
         <v>41800</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="8">
         <v>41799</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="8">
         <v>41797</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="8">
         <v>41796</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="8">
         <v>41795</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="8">
         <v>41794</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="8">
         <v>41793</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="8">
         <v>41792</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>6</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>6</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>6</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>8</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>12</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>8</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>6</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>8</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>6</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
     </row>
     <row r="17" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>2</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="6">
         <v>2</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="3">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="2">
         <f>(SUM(D17:D18)+SUM(D13:D15)+SUM(D9:D11)+SUM(D5:D7))</f>
         <v>69</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <f>D20-$D$20/12</f>
         <v>63.25</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="2">
         <f t="shared" ref="F20:P20" si="0">E20-$D$20/12</f>
         <v>57.5</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <f t="shared" si="0"/>
         <v>51.75</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <f t="shared" si="0"/>
         <v>40.25</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <f t="shared" si="0"/>
         <v>34.5</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="2">
         <f t="shared" si="0"/>
         <v>28.75</v>
       </c>
-      <c r="L20" s="3">
+      <c r="L20" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="M20" s="3">
+      <c r="M20" s="2">
         <f t="shared" si="0"/>
         <v>17.25</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20" s="2">
         <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="2">
         <f t="shared" si="0"/>
         <v>5.75</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="3">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="2">
         <f>D20</f>
         <v>69</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f>(SUM(E17:E18)+SUM(E13:E15)+SUM(E9:E11)+SUM(E5:E7))</f>
         <v>0</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <f t="shared" ref="F21:P21" si="1">(SUM(F17:F18)+SUM(F13:F15)+SUM(F9:F11)+SUM(F5:F7))</f>
         <v>0</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="2">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>

</xml_diff>